<commit_message>
timewarp for some example models
</commit_message>
<xml_diff>
--- a/doc/examples/calendar/calendar-working-hours.xlsx
+++ b/doc/examples/calendar/calendar-working-hours.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community\doc\user-guide\cookbook\calendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community\doc\examples\calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488B56DC-45A4-452E-A5D1-9F9D33C827FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="578" windowWidth="22725" windowHeight="11055" tabRatio="729" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="600" yWindow="-14130" windowWidth="27030" windowHeight="12405" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calendar bucket" sheetId="2" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t>name</t>
   </si>
@@ -99,12 +100,6 @@
     <t>Working hours</t>
   </si>
   <si>
-    <t>2000-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2030-12-31 00:00:00</t>
-  </si>
-  <si>
     <t>08:00:00</t>
   </si>
   <si>
@@ -117,12 +112,6 @@
     <t>12:59:59</t>
   </si>
   <si>
-    <t>2014-12-25 00:00:00</t>
-  </si>
-  <si>
-    <t>2014-12-26 00:00:00</t>
-  </si>
-  <si>
     <t>00:00:00</t>
   </si>
   <si>
@@ -144,9 +133,6 @@
     <t>My order</t>
   </si>
   <si>
-    <t>2014-12-27 12:00:00</t>
-  </si>
-  <si>
     <t>open</t>
   </si>
   <si>
@@ -168,9 +154,6 @@
     <t>fixed_time</t>
   </si>
   <si>
-    <t>2014-01-01 00:00:00</t>
-  </si>
-  <si>
     <t>currentdate</t>
   </si>
   <si>
@@ -197,11 +180,14 @@
   <si>
     <t>lead time</t>
   </si>
+  <si>
+    <t>2023-01-01  00:00:00 AM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,8 +217,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -326,6 +314,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -361,6 +366,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -536,20 +558,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -593,15 +615,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
+      <c r="B2" s="1">
+        <v>36526</v>
+      </c>
+      <c r="C2" s="1">
+        <v>47848</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -631,21 +653,21 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
+      <c r="B3" s="1">
+        <v>36526</v>
+      </c>
+      <c r="C3" s="1">
+        <v>47848</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -675,21 +697,21 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
+      <c r="B4" s="1">
+        <v>45285</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45286</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -719,10 +741,10 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -731,20 +753,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -755,15 +777,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -772,27 +794,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -800,9 +822,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -814,16 +836,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -834,24 +859,24 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -859,11 +884,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>38</v>
+      <c r="D2" s="1">
+        <v>45287.5</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -872,7 +897,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -881,23 +906,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -906,36 +931,36 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -944,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -953,16 +978,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -970,13 +995,13 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -984,7 +1009,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D2">
         <v>172800</v>
@@ -996,21 +1021,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1021,37 +1046,37 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -1063,24 +1088,24 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.53125" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1094,24 +1119,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E2">
         <v>172800</v>

</xml_diff>